<commit_message>
Primeira versão do 5W1H finalizada.
</commit_message>
<xml_diff>
--- a/Artefatos/5W1H/5W1H - Aplicativo para Ensino de Crianças.xlsx
+++ b/Artefatos/5W1H/5W1H - Aplicativo para Ensino de Crianças.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Aplicativo-para-Ensino-de-Criancas\Artefatos\5W1H\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC1E64F-8CF1-4E88-A4F1-408DADBF226C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F280C2C2-A053-4419-8C5B-1F86601F69FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1B06AB8-B0B0-4B88-8A80-3ABCD286D1B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>5W1H - Aplicativo para Ensino de Crianças</t>
   </si>
@@ -79,6 +79,33 @@
   </si>
   <si>
     <t>17/04/2021 a 30/04/2021</t>
+  </si>
+  <si>
+    <t>Tarcísio José Martins Ribeiro</t>
+  </si>
+  <si>
+    <t>Buscando material por meio de livros, artigos científicos e conteúdo coletado em meio eletrônico relevante.</t>
+  </si>
+  <si>
+    <t>Esclarecer e justificar os meios e técnicas que serão usados no desenvolvimento do protótipo.</t>
+  </si>
+  <si>
+    <t>Utilizando-se da linguagem UML para elaboração dos artefatos.</t>
+  </si>
+  <si>
+    <t>Utilizando ferramentas para prototipação de aplicações móveis, como Adobe XD.</t>
+  </si>
+  <si>
+    <t>Por meio de entrevistas com possíveis usuários, e análises de aplicações com o mesmo propósito que estão no mercado.</t>
+  </si>
+  <si>
+    <t>Definir de forma clara e objetiva quais serão os requisitos funcionais e não-funcionais do projeto, otimizando um futuro desenvolvimento.</t>
+  </si>
+  <si>
+    <t>Ilustrar os processos e diagramas do protótipo.</t>
+  </si>
+  <si>
+    <t>Entregar uma primeira visão das telas e ações do aplicativo.</t>
   </si>
 </sst>
 </file>
@@ -230,44 +257,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,32 +340,68 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,6 +412,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,468 +729,495 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0FB3F0-3E37-432B-A188-C59014A59767}">
   <dimension ref="C3:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:N11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="13" width="8.88671875" style="52"/>
+    <col min="14" max="14" width="8.88671875" style="52" customWidth="1"/>
+    <col min="15" max="16" width="8.88671875" style="52"/>
+    <col min="17" max="17" width="14.5546875" style="52" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="52"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="16"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="12"/>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="19"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="15"/>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="22"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="18"/>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8" t="s">
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="8" t="s">
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="8" t="s">
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8" t="s">
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8" t="s">
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="10"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="30"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="13"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="33"/>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="4"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="45"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="48"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="7"/>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="43"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="48"/>
+    </row>
+    <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="51"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="2" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="S12" s="3"/>
-      <c r="T12" s="4"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="45"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="7"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="48"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C14" s="35"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="7"/>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="43"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="48"/>
+    </row>
+    <row r="15" spans="3:20" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="51"/>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="2" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="20"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="S16" s="3"/>
-      <c r="T16" s="4"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="45"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="48"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="48"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="43"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="51"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="2" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="20"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="S20" s="3"/>
-      <c r="T20" s="4"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="45"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="7"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="48"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="48"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C23" s="38"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="43"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="F6:H7"/>
     <mergeCell ref="C6:E7"/>
     <mergeCell ref="O20:Q23"/>
     <mergeCell ref="R20:T23"/>
@@ -1152,21 +1233,22 @@
     <mergeCell ref="R16:T19"/>
     <mergeCell ref="L8:N11"/>
     <mergeCell ref="I12:K15"/>
+    <mergeCell ref="C8:E11"/>
+    <mergeCell ref="C12:E15"/>
+    <mergeCell ref="C16:E19"/>
+    <mergeCell ref="C20:E23"/>
+    <mergeCell ref="C3:T5"/>
+    <mergeCell ref="F8:H11"/>
+    <mergeCell ref="F12:H15"/>
+    <mergeCell ref="F16:H19"/>
+    <mergeCell ref="F20:H23"/>
+    <mergeCell ref="I8:K11"/>
     <mergeCell ref="L12:N15"/>
     <mergeCell ref="I16:K19"/>
     <mergeCell ref="L16:N19"/>
     <mergeCell ref="I20:K23"/>
     <mergeCell ref="L20:N23"/>
-    <mergeCell ref="F8:H11"/>
-    <mergeCell ref="F12:H15"/>
-    <mergeCell ref="F16:H19"/>
-    <mergeCell ref="F20:H23"/>
-    <mergeCell ref="I8:K11"/>
-    <mergeCell ref="C8:E11"/>
-    <mergeCell ref="C12:E15"/>
-    <mergeCell ref="C16:E19"/>
-    <mergeCell ref="C20:E23"/>
-    <mergeCell ref="C3:T5"/>
+    <mergeCell ref="F6:H7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>